<commit_message>
Selection du meilleur budget sur un portefeuille de projets
</commit_message>
<xml_diff>
--- a/26. Excel - Recherche opérationnelle linéaire/53 - PROJET - SELECTION DE PROJETS SOUS CONTRAINTES/Copy of Capbudget.xlsx
+++ b/26. Excel - Recherche opérationnelle linéaire/53 - PROJET - SELECTION DE PROJETS SOUS CONTRAINTES/Copy of Capbudget.xlsx
@@ -9,204 +9,204 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="252" yWindow="180" windowWidth="11628" windowHeight="5976"/>
+    <workbookView xWindow="252" yWindow="180" windowWidth="11628" windowHeight="5976" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="basic model" sheetId="1" r:id="rId1"/>
-    <sheet name="At most 4 of P1-P10" sheetId="5" r:id="rId2"/>
-    <sheet name="tolerance .5" sheetId="6" r:id="rId3"/>
-    <sheet name="If 3 then 4" sheetId="4" r:id="rId4"/>
+    <sheet name="Au PLUS 4 entre P1 a P10" sheetId="5" r:id="rId2"/>
+    <sheet name="Si PROJET3 alors PROJET4" sheetId="4" r:id="rId3"/>
+    <sheet name="tolerance .5" sheetId="6" r:id="rId4"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="doit" localSheetId="1">'At most 4 of P1-P10'!$A$6:$A$25</definedName>
-    <definedName name="doit" localSheetId="3">'If 3 then 4'!$A$6:$A$25</definedName>
-    <definedName name="doit" localSheetId="2">'tolerance .5'!$A$6:$A$25</definedName>
+    <definedName name="doit" localSheetId="1">'Au PLUS 4 entre P1 a P10'!$A$6:$A$25</definedName>
+    <definedName name="doit" localSheetId="2">'Si PROJET3 alors PROJET4'!$A$6:$A$25</definedName>
+    <definedName name="doit" localSheetId="3">'tolerance .5'!$A$6:$A$25</definedName>
     <definedName name="doit">'basic model'!$A$6:$A$25</definedName>
-    <definedName name="NPV" localSheetId="1">'At most 4 of P1-P10'!$C$6:$C$25</definedName>
-    <definedName name="NPV" localSheetId="3">'If 3 then 4'!$C$6:$C$25</definedName>
-    <definedName name="NPV" localSheetId="2">'tolerance .5'!$C$6:$C$25</definedName>
+    <definedName name="NPV" localSheetId="1">'Au PLUS 4 entre P1 a P10'!$C$6:$C$25</definedName>
+    <definedName name="NPV" localSheetId="2">'Si PROJET3 alors PROJET4'!$C$6:$C$25</definedName>
+    <definedName name="NPV" localSheetId="3">'tolerance .5'!$C$6:$C$25</definedName>
     <definedName name="NPV">'basic model'!$C$6:$C$25</definedName>
-    <definedName name="solver_adj" localSheetId="1" hidden="1">'At most 4 of P1-P10'!$A$6:$A$25</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">'Au PLUS 4 entre P1 a P10'!$A$6:$A$25</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'basic model'!$A$6:$A$25</definedName>
-    <definedName name="solver_adj" localSheetId="3" hidden="1">'If 3 then 4'!$A$6:$A$25</definedName>
-    <definedName name="solver_adj" localSheetId="2" hidden="1">'tolerance .5'!$A$6:$A$25</definedName>
+    <definedName name="solver_adj" localSheetId="2" hidden="1">'Si PROJET3 alors PROJET4'!$A$6:$A$25</definedName>
+    <definedName name="solver_adj" localSheetId="3" hidden="1">'tolerance .5'!$A$6:$A$25</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="3" hidden="1">0.0001</definedName>
-    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_eng" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_ibd" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_ibd" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ibd" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_ibd" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_ibd" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_itr" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_itr" localSheetId="3" hidden="1">100</definedName>
-    <definedName name="solver_itr" localSheetId="2" hidden="1">100</definedName>
-    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'At most 4 of P1-P10'!$E$2:$J$2</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">'Au PLUS 4 entre P1 a P10'!$E$2:$J$2</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'basic model'!$E$2:$J$2</definedName>
-    <definedName name="solver_lhs1" localSheetId="3" hidden="1">'If 3 then 4'!$E$2:$J$2</definedName>
-    <definedName name="solver_lhs1" localSheetId="2" hidden="1">'tolerance .5'!$E$2:$J$2</definedName>
-    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'At most 4 of P1-P10'!$L$8</definedName>
+    <definedName name="solver_lhs1" localSheetId="2" hidden="1">'Si PROJET3 alors PROJET4'!$E$2:$J$2</definedName>
+    <definedName name="solver_lhs1" localSheetId="3" hidden="1">'tolerance .5'!$E$2:$J$2</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">'Au PLUS 4 entre P1 a P10'!$L$8</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">'basic model'!$A$6:$A$25</definedName>
-    <definedName name="solver_lhs2" localSheetId="3" hidden="1">'If 3 then 4'!$L$9</definedName>
-    <definedName name="solver_lhs2" localSheetId="2" hidden="1">'tolerance .5'!$A$6:$A$25</definedName>
-    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'At most 4 of P1-P10'!$A$6:$A$25</definedName>
-    <definedName name="solver_lhs3" localSheetId="3" hidden="1">'If 3 then 4'!$A$6:$A$25</definedName>
+    <definedName name="solver_lhs2" localSheetId="2" hidden="1">'Si PROJET3 alors PROJET4'!$L$9</definedName>
+    <definedName name="solver_lhs2" localSheetId="3" hidden="1">'tolerance .5'!$A$6:$A$25</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">'Au PLUS 4 entre P1 a P10'!$A$6:$A$25</definedName>
+    <definedName name="solver_lhs3" localSheetId="2" hidden="1">'Si PROJET3 alors PROJET4'!$A$6:$A$25</definedName>
     <definedName name="solver_lin" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_lin" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_lin" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_lin" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_lin" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_lva" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_lva" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_lva" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_lva" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_lva" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_mip" localSheetId="1" hidden="1">5000</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">5000</definedName>
+    <definedName name="solver_mip" localSheetId="2" hidden="1">5000</definedName>
     <definedName name="solver_mip" localSheetId="3" hidden="1">5000</definedName>
-    <definedName name="solver_mip" localSheetId="2" hidden="1">5000</definedName>
     <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="3" hidden="1">30</definedName>
-    <definedName name="solver_mni" localSheetId="2" hidden="1">30</definedName>
     <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="3" hidden="1">0.075</definedName>
-    <definedName name="solver_mrt" localSheetId="2" hidden="1">0.075</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_neg" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_nod" localSheetId="1" hidden="1">5000</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">5000</definedName>
+    <definedName name="solver_nod" localSheetId="2" hidden="1">5000</definedName>
     <definedName name="solver_nod" localSheetId="3" hidden="1">5000</definedName>
-    <definedName name="solver_nod" localSheetId="2" hidden="1">5000</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_num" localSheetId="3" hidden="1">3</definedName>
-    <definedName name="solver_num" localSheetId="2" hidden="1">2</definedName>
+    <definedName name="solver_num" localSheetId="2" hidden="1">3</definedName>
+    <definedName name="solver_num" localSheetId="3" hidden="1">2</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_ofx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_ofx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ofx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_ofx" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_ofx" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_opt" localSheetId="1" hidden="1">'At most 4 of P1-P10'!$B$2</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">'Au PLUS 4 entre P1 a P10'!$B$2</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'basic model'!$B$2</definedName>
-    <definedName name="solver_opt" localSheetId="3" hidden="1">'If 3 then 4'!$B$2</definedName>
-    <definedName name="solver_opt" localSheetId="2" hidden="1">'tolerance .5'!$B$2</definedName>
+    <definedName name="solver_opt" localSheetId="2" hidden="1">'Si PROJET3 alors PROJET4'!$B$2</definedName>
+    <definedName name="solver_opt" localSheetId="3" hidden="1">'tolerance .5'!$B$2</definedName>
     <definedName name="solver_piv" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_piv" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_piv" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_piv" localSheetId="3" hidden="1">0.000001</definedName>
-    <definedName name="solver_piv" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="3" hidden="1">0.000001</definedName>
-    <definedName name="solver_pre" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_pro" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_pro" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_pro" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_pro" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_pro" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rbv" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rbv" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rbv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_red" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_red" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_red" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_red" localSheetId="3" hidden="1">0.000001</definedName>
-    <definedName name="solver_red" localSheetId="2" hidden="1">0.000001</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel1" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">5</definedName>
-    <definedName name="solver_rel2" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_rel2" localSheetId="2" hidden="1">5</definedName>
+    <definedName name="solver_rel2" localSheetId="2" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="3" hidden="1">5</definedName>
     <definedName name="solver_rel3" localSheetId="1" hidden="1">5</definedName>
-    <definedName name="solver_rel3" localSheetId="3" hidden="1">5</definedName>
+    <definedName name="solver_rel3" localSheetId="2" hidden="1">5</definedName>
     <definedName name="solver_reo" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_reo" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_reo" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_reo" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_reo" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rep" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rep" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rep" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rep" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_rep" localSheetId="2" hidden="1">2</definedName>
-    <definedName name="solver_rhs1" localSheetId="1" hidden="1">'At most 4 of P1-P10'!$E$4:$J$4</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">'Au PLUS 4 entre P1 a P10'!$E$4:$J$4</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">'basic model'!$E$4:$J$4</definedName>
-    <definedName name="solver_rhs1" localSheetId="3" hidden="1">'If 3 then 4'!$E$4:$J$4</definedName>
-    <definedName name="solver_rhs1" localSheetId="2" hidden="1">'tolerance .5'!$E$4:$J$4</definedName>
-    <definedName name="solver_rhs2" localSheetId="1" hidden="1">'At most 4 of P1-P10'!$L$10</definedName>
+    <definedName name="solver_rhs1" localSheetId="2" hidden="1">'Si PROJET3 alors PROJET4'!$E$4:$J$4</definedName>
+    <definedName name="solver_rhs1" localSheetId="3" hidden="1">'tolerance .5'!$E$4:$J$4</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">'Au PLUS 4 entre P1 a P10'!$L$10</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">"binary"</definedName>
-    <definedName name="solver_rhs2" localSheetId="3" hidden="1">'If 3 then 4'!$L$12</definedName>
-    <definedName name="solver_rhs2" localSheetId="2" hidden="1">binary</definedName>
+    <definedName name="solver_rhs2" localSheetId="2" hidden="1">'Si PROJET3 alors PROJET4'!$L$12</definedName>
+    <definedName name="solver_rhs2" localSheetId="3" hidden="1">binary</definedName>
     <definedName name="solver_rhs3" localSheetId="1" hidden="1">"binary"</definedName>
-    <definedName name="solver_rhs3" localSheetId="3" hidden="1">binary</definedName>
+    <definedName name="solver_rhs3" localSheetId="2" hidden="1">"binary"</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_scl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_scl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_sho" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="3" hidden="1">100</definedName>
-    <definedName name="solver_ssz" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_std" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_std" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_std" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_std" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_std" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_tim" localSheetId="3" hidden="1">100</definedName>
-    <definedName name="solver_tim" localSheetId="2" hidden="1">100</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.0005</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.0005</definedName>
+    <definedName name="solver_tol" localSheetId="2" hidden="1">0.005</definedName>
     <definedName name="solver_tol" localSheetId="3" hidden="1">0.005</definedName>
-    <definedName name="solver_tol" localSheetId="2" hidden="1">0.005</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="3" hidden="1">1</definedName>
-    <definedName name="solver_typ" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="3" hidden="1">0</definedName>
-    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="2" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="3" hidden="1">2</definedName>
-    <definedName name="solver_ver" localSheetId="2" hidden="1">2</definedName>
   </definedNames>
   <calcPr calcId="162913" iterate="1" iterateCount="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="42">
   <si>
     <t>Project 1</t>
   </si>
@@ -330,12 +330,15 @@
   <si>
     <t>Suite au click sur le solveur, le solveur nous dit combien on va investir par années, en calculant à l'aide des vars de décision "DO IT " qui sont binaires</t>
   </si>
+  <si>
+    <t>Ce que rapporte chaque projets en millions de $</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -351,8 +354,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -389,6 +399,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -402,7 +424,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -413,6 +435,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,6 +711,170 @@
           <a:r>
             <a:rPr lang="fr-FR"/>
             <a:t>Par exemple, au cours de l'année 1, jusqu'à 2,5 milliards de dollars en capital et 900 programmeurs sont disponibles</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>33867</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>118533</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>448734</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8466667" y="2480733"/>
+          <a:ext cx="4800600" cy="2785534"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>Ici, </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>on a le même problème</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t> que dans l'onglet un, sauf qu'on ajoute la contrainte qu'on ne veut choisir que au plus 4 projets maximum entre les projets 1 à 10 .</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="fr-FR" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t>Du coup, on investit moins mais on respecte bien la contrainte, on voit que le solveur choisit le projet 3, 7, 8 , alors que dans le premier onglet, il en choisit beaucoup plus de projet entre  les P1 et P10</a:t>
+          </a:r>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>129540</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>617220</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1"/>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8458200" y="601980"/>
+          <a:ext cx="3611880" cy="2773680"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>Ici, on a une nouvelle contrainte,</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100"/>
+            <a:t>Si</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" baseline="0"/>
+            <a:t> on choisit le projet3, alors le projet 4 doit être choisi !</a:t>
           </a:r>
           <a:endParaRPr lang="fr-FR" sz="1100"/>
         </a:p>
@@ -983,10 +1172,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J32"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -1114,25 +1303,25 @@
       <c r="B6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="9">
         <v>928</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="10">
         <v>398</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="10">
         <v>180</v>
       </c>
-      <c r="G6" s="1">
+      <c r="G6" s="10">
         <v>368</v>
       </c>
-      <c r="H6" s="1">
+      <c r="H6" s="3">
         <v>111</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="3">
         <v>108</v>
       </c>
-      <c r="J6" s="1">
+      <c r="J6" s="3">
         <v>123</v>
       </c>
     </row>
@@ -1143,25 +1332,25 @@
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="9">
         <v>908</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="10">
         <v>151</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="10">
         <v>269</v>
       </c>
-      <c r="G7" s="1">
+      <c r="G7" s="10">
         <v>248</v>
       </c>
-      <c r="H7" s="1">
+      <c r="H7" s="3">
         <v>139</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="3">
         <v>86</v>
       </c>
-      <c r="J7" s="1">
+      <c r="J7" s="3">
         <v>83</v>
       </c>
     </row>
@@ -1172,25 +1361,25 @@
       <c r="B8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="9">
         <v>801</v>
       </c>
-      <c r="E8" s="1">
+      <c r="E8" s="10">
         <v>129</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="10">
         <v>189</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="10">
         <v>308</v>
       </c>
-      <c r="H8" s="1">
+      <c r="H8" s="3">
         <v>56</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="3">
         <v>61</v>
       </c>
-      <c r="J8" s="1">
+      <c r="J8" s="3">
         <v>23</v>
       </c>
     </row>
@@ -1201,25 +1390,25 @@
       <c r="B9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="9">
         <v>543</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="10">
         <v>275</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="10">
         <v>218</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="10">
         <v>220</v>
       </c>
-      <c r="H9" s="1">
+      <c r="H9" s="3">
         <v>54</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="3">
         <v>70</v>
       </c>
-      <c r="J9" s="1">
+      <c r="J9" s="3">
         <v>59</v>
       </c>
     </row>
@@ -1230,25 +1419,25 @@
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="9">
         <v>944</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="10">
         <v>291</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="10">
         <v>252</v>
       </c>
-      <c r="G10" s="1">
+      <c r="G10" s="10">
         <v>228</v>
       </c>
-      <c r="H10" s="1">
+      <c r="H10" s="3">
         <v>123</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="3">
         <v>141</v>
       </c>
-      <c r="J10" s="1">
+      <c r="J10" s="3">
         <v>70</v>
       </c>
     </row>
@@ -1259,25 +1448,25 @@
       <c r="B11" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="9">
         <v>848</v>
       </c>
-      <c r="E11" s="1">
+      <c r="E11" s="10">
         <v>80</v>
       </c>
-      <c r="F11" s="1">
+      <c r="F11" s="10">
         <v>283</v>
       </c>
-      <c r="G11" s="1">
+      <c r="G11" s="10">
         <v>285</v>
       </c>
-      <c r="H11" s="1">
+      <c r="H11" s="3">
         <v>119</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="3">
         <v>84</v>
       </c>
-      <c r="J11" s="1">
+      <c r="J11" s="3">
         <v>37</v>
       </c>
     </row>
@@ -1288,25 +1477,25 @@
       <c r="B12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="9">
         <v>545</v>
       </c>
-      <c r="E12" s="1">
+      <c r="E12" s="10">
         <v>203</v>
       </c>
-      <c r="F12" s="1">
+      <c r="F12" s="10">
         <v>220</v>
       </c>
-      <c r="G12" s="1">
+      <c r="G12" s="10">
         <v>77</v>
       </c>
-      <c r="H12" s="1">
+      <c r="H12" s="3">
         <v>54</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="3">
         <v>44</v>
       </c>
-      <c r="J12" s="1">
+      <c r="J12" s="3">
         <v>42</v>
       </c>
     </row>
@@ -1317,25 +1506,25 @@
       <c r="B13" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="9">
         <v>808</v>
       </c>
-      <c r="E13" s="1">
+      <c r="E13" s="10">
         <v>150</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="10">
         <v>113</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="10">
         <v>143</v>
       </c>
-      <c r="H13" s="1">
+      <c r="H13" s="3">
         <v>67</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="3">
         <v>101</v>
       </c>
-      <c r="J13" s="1">
+      <c r="J13" s="3">
         <v>43</v>
       </c>
     </row>
@@ -1346,25 +1535,25 @@
       <c r="B14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="9">
         <v>638</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="10">
         <v>282</v>
       </c>
-      <c r="F14" s="1">
+      <c r="F14" s="10">
         <v>141</v>
       </c>
-      <c r="G14" s="1">
+      <c r="G14" s="10">
         <v>160</v>
       </c>
-      <c r="H14" s="1">
+      <c r="H14" s="3">
         <v>37</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14" s="3">
         <v>55</v>
       </c>
-      <c r="J14" s="1">
+      <c r="J14" s="3">
         <v>64</v>
       </c>
     </row>
@@ -1375,25 +1564,25 @@
       <c r="B15" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="9">
         <v>841</v>
       </c>
-      <c r="E15" s="1">
+      <c r="E15" s="10">
         <v>214</v>
       </c>
-      <c r="F15" s="1">
+      <c r="F15" s="10">
         <v>254</v>
       </c>
-      <c r="G15" s="1">
+      <c r="G15" s="10">
         <v>355</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="3">
         <v>130</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="3">
         <v>72</v>
       </c>
-      <c r="J15" s="1">
+      <c r="J15" s="3">
         <v>62</v>
       </c>
     </row>
@@ -1404,25 +1593,25 @@
       <c r="B16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="9">
         <v>664</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="10">
         <v>224</v>
       </c>
-      <c r="F16" s="1">
+      <c r="F16" s="10">
         <v>271</v>
       </c>
-      <c r="G16" s="1">
+      <c r="G16" s="10">
         <v>130</v>
       </c>
-      <c r="H16" s="1">
+      <c r="H16" s="3">
         <v>51</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="3">
         <v>79</v>
       </c>
-      <c r="J16" s="1">
+      <c r="J16" s="3">
         <v>58</v>
       </c>
     </row>
@@ -1433,25 +1622,25 @@
       <c r="B17" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="9">
         <v>546</v>
       </c>
-      <c r="E17" s="1">
+      <c r="E17" s="10">
         <v>225</v>
       </c>
-      <c r="F17" s="1">
+      <c r="F17" s="10">
         <v>150</v>
       </c>
-      <c r="G17" s="1">
+      <c r="G17" s="10">
         <v>33</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H17" s="3">
         <v>35</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17" s="3">
         <v>107</v>
       </c>
-      <c r="J17" s="1">
+      <c r="J17" s="3">
         <v>63</v>
       </c>
     </row>
@@ -1462,25 +1651,25 @@
       <c r="B18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="9">
         <v>699</v>
       </c>
-      <c r="E18" s="1">
+      <c r="E18" s="10">
         <v>101</v>
       </c>
-      <c r="F18" s="1">
+      <c r="F18" s="10">
         <v>218</v>
       </c>
-      <c r="G18" s="1">
+      <c r="G18" s="10">
         <v>272</v>
       </c>
-      <c r="H18" s="1">
+      <c r="H18" s="3">
         <v>43</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18" s="3">
         <v>90</v>
       </c>
-      <c r="J18" s="1">
+      <c r="J18" s="3">
         <v>71</v>
       </c>
     </row>
@@ -1491,25 +1680,25 @@
       <c r="B19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="9">
         <v>599</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="10">
         <v>255</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="10">
         <v>202</v>
       </c>
-      <c r="G19" s="1">
+      <c r="G19" s="10">
         <v>70</v>
       </c>
-      <c r="H19" s="1">
+      <c r="H19" s="3">
         <v>3</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19" s="3">
         <v>75</v>
       </c>
-      <c r="J19" s="1">
+      <c r="J19" s="3">
         <v>83</v>
       </c>
     </row>
@@ -1520,25 +1709,25 @@
       <c r="B20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="9">
         <v>903</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="10">
         <v>228</v>
       </c>
-      <c r="F20" s="1">
+      <c r="F20" s="10">
         <v>351</v>
       </c>
-      <c r="G20" s="1">
+      <c r="G20" s="10">
         <v>240</v>
       </c>
-      <c r="H20" s="1">
+      <c r="H20" s="3">
         <v>60</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20" s="3">
         <v>93</v>
       </c>
-      <c r="J20" s="1">
+      <c r="J20" s="3">
         <v>80</v>
       </c>
     </row>
@@ -1549,25 +1738,25 @@
       <c r="B21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="9">
         <v>859</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="10">
         <v>303</v>
       </c>
-      <c r="F21" s="1">
+      <c r="F21" s="10">
         <v>173</v>
       </c>
-      <c r="G21" s="1">
+      <c r="G21" s="10">
         <v>431</v>
       </c>
-      <c r="H21" s="1">
+      <c r="H21" s="3">
         <v>60</v>
       </c>
-      <c r="I21" s="1">
+      <c r="I21" s="3">
         <v>90</v>
       </c>
-      <c r="J21" s="1">
+      <c r="J21" s="3">
         <v>41</v>
       </c>
     </row>
@@ -1578,25 +1767,25 @@
       <c r="B22" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="9">
         <v>748</v>
       </c>
-      <c r="E22" s="1">
+      <c r="E22" s="10">
         <v>133</v>
       </c>
-      <c r="F22" s="1">
+      <c r="F22" s="10">
         <v>427</v>
       </c>
-      <c r="G22" s="1">
+      <c r="G22" s="10">
         <v>220</v>
       </c>
-      <c r="H22" s="1">
+      <c r="H22" s="3">
         <v>59</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I22" s="3">
         <v>40</v>
       </c>
-      <c r="J22" s="1">
+      <c r="J22" s="3">
         <v>39</v>
       </c>
     </row>
@@ -1607,25 +1796,25 @@
       <c r="B23" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="9">
         <v>668</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="10">
         <v>197</v>
       </c>
-      <c r="F23" s="1">
+      <c r="F23" s="10">
         <v>98</v>
       </c>
-      <c r="G23" s="1">
+      <c r="G23" s="10">
         <v>214</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23" s="3">
         <v>95</v>
       </c>
-      <c r="I23" s="1">
+      <c r="I23" s="3">
         <v>96</v>
       </c>
-      <c r="J23" s="1">
+      <c r="J23" s="3">
         <v>74</v>
       </c>
     </row>
@@ -1636,25 +1825,25 @@
       <c r="B24" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="9">
         <v>888</v>
       </c>
-      <c r="E24" s="1">
+      <c r="E24" s="10">
         <v>313</v>
       </c>
-      <c r="F24" s="1">
+      <c r="F24" s="10">
         <v>278</v>
       </c>
-      <c r="G24" s="1">
+      <c r="G24" s="10">
         <v>291</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24" s="3">
         <v>66</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I24" s="3">
         <v>75</v>
       </c>
-      <c r="J24" s="1">
+      <c r="J24" s="3">
         <v>74</v>
       </c>
     </row>
@@ -1665,25 +1854,25 @@
       <c r="B25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="9">
         <v>655</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="10">
         <v>152</v>
       </c>
-      <c r="F25" s="1">
+      <c r="F25" s="10">
         <v>211</v>
       </c>
-      <c r="G25" s="1">
+      <c r="G25" s="10">
         <v>134</v>
       </c>
-      <c r="H25" s="1">
+      <c r="H25" s="3">
         <v>85</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I25" s="3">
         <v>59</v>
       </c>
-      <c r="J25" s="1">
+      <c r="J25" s="3">
         <v>70</v>
       </c>
     </row>
@@ -1715,6 +1904,12 @@
       <c r="A32" s="7"/>
       <c r="B32" s="1" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="8"/>
+      <c r="B33" s="1" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -1730,7 +1925,7 @@
   <dimension ref="A1:O25"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="J4" sqref="E4:J4"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2471,6 +2666,740 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N25" sqref="N25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.109375" style="1"/>
+    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.109375" style="1"/>
+    <col min="5" max="5" width="11.5546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="1" customWidth="1"/>
+    <col min="7" max="8" width="11.44140625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.44140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="5.44140625" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B2" s="1">
+        <f>SUMPRODUCT(doit,NPV)</f>
+        <v>9157</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="1">
+        <f t="shared" ref="E2:J2" si="0">SUMPRODUCT(doit,E6:E25)</f>
+        <v>2444</v>
+      </c>
+      <c r="F2" s="1">
+        <f t="shared" si="0"/>
+        <v>2760</v>
+      </c>
+      <c r="G2" s="1">
+        <f t="shared" si="0"/>
+        <v>2837</v>
+      </c>
+      <c r="H2" s="1">
+        <f t="shared" si="0"/>
+        <v>866</v>
+      </c>
+      <c r="I2" s="1">
+        <f t="shared" si="0"/>
+        <v>895</v>
+      </c>
+      <c r="J2" s="1">
+        <f t="shared" si="0"/>
+        <v>659</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="1">
+        <v>2500</v>
+      </c>
+      <c r="F4" s="1">
+        <v>2800</v>
+      </c>
+      <c r="G4" s="1">
+        <v>2900</v>
+      </c>
+      <c r="H4" s="1">
+        <v>900</v>
+      </c>
+      <c r="I4" s="1">
+        <v>900</v>
+      </c>
+      <c r="J4" s="1">
+        <v>900</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1">
+        <v>928</v>
+      </c>
+      <c r="E6" s="1">
+        <v>398</v>
+      </c>
+      <c r="F6" s="1">
+        <v>180</v>
+      </c>
+      <c r="G6" s="1">
+        <v>368</v>
+      </c>
+      <c r="H6" s="1">
+        <v>111</v>
+      </c>
+      <c r="I6" s="1">
+        <v>108</v>
+      </c>
+      <c r="J6" s="1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="1">
+        <v>908</v>
+      </c>
+      <c r="E7" s="1">
+        <v>151</v>
+      </c>
+      <c r="F7" s="1">
+        <v>269</v>
+      </c>
+      <c r="G7" s="1">
+        <v>248</v>
+      </c>
+      <c r="H7" s="1">
+        <v>139</v>
+      </c>
+      <c r="I7" s="1">
+        <v>86</v>
+      </c>
+      <c r="J7" s="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>801</v>
+      </c>
+      <c r="E8" s="1">
+        <v>129</v>
+      </c>
+      <c r="F8" s="1">
+        <v>189</v>
+      </c>
+      <c r="G8" s="1">
+        <v>308</v>
+      </c>
+      <c r="H8" s="1">
+        <v>56</v>
+      </c>
+      <c r="I8" s="1">
+        <v>61</v>
+      </c>
+      <c r="J8" s="1">
+        <v>23</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="1">
+        <v>543</v>
+      </c>
+      <c r="E9" s="1">
+        <v>275</v>
+      </c>
+      <c r="F9" s="1">
+        <v>218</v>
+      </c>
+      <c r="G9" s="1">
+        <v>220</v>
+      </c>
+      <c r="H9" s="1">
+        <v>54</v>
+      </c>
+      <c r="I9" s="1">
+        <v>70</v>
+      </c>
+      <c r="J9" s="1">
+        <v>59</v>
+      </c>
+      <c r="L9" s="1">
+        <f>A8</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="1">
+        <v>944</v>
+      </c>
+      <c r="E10" s="1">
+        <v>291</v>
+      </c>
+      <c r="F10" s="1">
+        <v>252</v>
+      </c>
+      <c r="G10" s="1">
+        <v>228</v>
+      </c>
+      <c r="H10" s="1">
+        <v>123</v>
+      </c>
+      <c r="I10" s="1">
+        <v>141</v>
+      </c>
+      <c r="J10" s="1">
+        <v>70</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="1">
+        <v>848</v>
+      </c>
+      <c r="E11" s="1">
+        <v>80</v>
+      </c>
+      <c r="F11" s="1">
+        <v>283</v>
+      </c>
+      <c r="G11" s="1">
+        <v>285</v>
+      </c>
+      <c r="H11" s="1">
+        <v>119</v>
+      </c>
+      <c r="I11" s="1">
+        <v>84</v>
+      </c>
+      <c r="J11" s="1">
+        <v>37</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="1">
+        <v>545</v>
+      </c>
+      <c r="E12" s="1">
+        <v>203</v>
+      </c>
+      <c r="F12" s="1">
+        <v>220</v>
+      </c>
+      <c r="G12" s="1">
+        <v>77</v>
+      </c>
+      <c r="H12" s="1">
+        <v>54</v>
+      </c>
+      <c r="I12" s="1">
+        <v>44</v>
+      </c>
+      <c r="J12" s="1">
+        <v>42</v>
+      </c>
+      <c r="L12" s="1">
+        <f>A9</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="1">
+        <v>808</v>
+      </c>
+      <c r="E13" s="1">
+        <v>150</v>
+      </c>
+      <c r="F13" s="1">
+        <v>113</v>
+      </c>
+      <c r="G13" s="1">
+        <v>143</v>
+      </c>
+      <c r="H13" s="1">
+        <v>67</v>
+      </c>
+      <c r="I13" s="1">
+        <v>101</v>
+      </c>
+      <c r="J13" s="1">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="1">
+        <v>638</v>
+      </c>
+      <c r="E14" s="1">
+        <v>282</v>
+      </c>
+      <c r="F14" s="1">
+        <v>141</v>
+      </c>
+      <c r="G14" s="1">
+        <v>160</v>
+      </c>
+      <c r="H14" s="1">
+        <v>37</v>
+      </c>
+      <c r="I14" s="1">
+        <v>55</v>
+      </c>
+      <c r="J14" s="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>0</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="1">
+        <v>841</v>
+      </c>
+      <c r="E15" s="1">
+        <v>214</v>
+      </c>
+      <c r="F15" s="1">
+        <v>254</v>
+      </c>
+      <c r="G15" s="1">
+        <v>355</v>
+      </c>
+      <c r="H15" s="1">
+        <v>130</v>
+      </c>
+      <c r="I15" s="1">
+        <v>72</v>
+      </c>
+      <c r="J15" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>0</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="1">
+        <v>664</v>
+      </c>
+      <c r="E16" s="1">
+        <v>224</v>
+      </c>
+      <c r="F16" s="1">
+        <v>271</v>
+      </c>
+      <c r="G16" s="1">
+        <v>130</v>
+      </c>
+      <c r="H16" s="1">
+        <v>51</v>
+      </c>
+      <c r="I16" s="1">
+        <v>79</v>
+      </c>
+      <c r="J16" s="1">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1">
+        <v>546</v>
+      </c>
+      <c r="E17" s="1">
+        <v>225</v>
+      </c>
+      <c r="F17" s="1">
+        <v>150</v>
+      </c>
+      <c r="G17" s="1">
+        <v>33</v>
+      </c>
+      <c r="H17" s="1">
+        <v>35</v>
+      </c>
+      <c r="I17" s="1">
+        <v>107</v>
+      </c>
+      <c r="J17" s="1">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>0</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="1">
+        <v>699</v>
+      </c>
+      <c r="E18" s="1">
+        <v>101</v>
+      </c>
+      <c r="F18" s="1">
+        <v>218</v>
+      </c>
+      <c r="G18" s="1">
+        <v>272</v>
+      </c>
+      <c r="H18" s="1">
+        <v>43</v>
+      </c>
+      <c r="I18" s="1">
+        <v>90</v>
+      </c>
+      <c r="J18" s="1">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>0</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="1">
+        <v>599</v>
+      </c>
+      <c r="E19" s="1">
+        <v>255</v>
+      </c>
+      <c r="F19" s="1">
+        <v>202</v>
+      </c>
+      <c r="G19" s="1">
+        <v>70</v>
+      </c>
+      <c r="H19" s="1">
+        <v>3</v>
+      </c>
+      <c r="I19" s="1">
+        <v>75</v>
+      </c>
+      <c r="J19" s="1">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>1</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="1">
+        <v>903</v>
+      </c>
+      <c r="E20" s="1">
+        <v>228</v>
+      </c>
+      <c r="F20" s="1">
+        <v>351</v>
+      </c>
+      <c r="G20" s="1">
+        <v>240</v>
+      </c>
+      <c r="H20" s="1">
+        <v>60</v>
+      </c>
+      <c r="I20" s="1">
+        <v>93</v>
+      </c>
+      <c r="J20" s="1">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>1</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="1">
+        <v>859</v>
+      </c>
+      <c r="E21" s="1">
+        <v>303</v>
+      </c>
+      <c r="F21" s="1">
+        <v>173</v>
+      </c>
+      <c r="G21" s="1">
+        <v>431</v>
+      </c>
+      <c r="H21" s="1">
+        <v>60</v>
+      </c>
+      <c r="I21" s="1">
+        <v>90</v>
+      </c>
+      <c r="J21" s="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>1</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="1">
+        <v>748</v>
+      </c>
+      <c r="E22" s="1">
+        <v>133</v>
+      </c>
+      <c r="F22" s="1">
+        <v>427</v>
+      </c>
+      <c r="G22" s="1">
+        <v>220</v>
+      </c>
+      <c r="H22" s="1">
+        <v>59</v>
+      </c>
+      <c r="I22" s="1">
+        <v>40</v>
+      </c>
+      <c r="J22" s="1">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>1</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C23" s="1">
+        <v>668</v>
+      </c>
+      <c r="E23" s="1">
+        <v>197</v>
+      </c>
+      <c r="F23" s="1">
+        <v>98</v>
+      </c>
+      <c r="G23" s="1">
+        <v>214</v>
+      </c>
+      <c r="H23" s="1">
+        <v>95</v>
+      </c>
+      <c r="I23" s="1">
+        <v>96</v>
+      </c>
+      <c r="J23" s="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>1</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="1">
+        <v>888</v>
+      </c>
+      <c r="E24" s="1">
+        <v>313</v>
+      </c>
+      <c r="F24" s="1">
+        <v>278</v>
+      </c>
+      <c r="G24" s="1">
+        <v>291</v>
+      </c>
+      <c r="H24" s="1">
+        <v>66</v>
+      </c>
+      <c r="I24" s="1">
+        <v>75</v>
+      </c>
+      <c r="J24" s="1">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>0</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="1">
+        <v>655</v>
+      </c>
+      <c r="E25" s="1">
+        <v>152</v>
+      </c>
+      <c r="F25" s="1">
+        <v>211</v>
+      </c>
+      <c r="G25" s="1">
+        <v>134</v>
+      </c>
+      <c r="H25" s="1">
+        <v>85</v>
+      </c>
+      <c r="I25" s="1">
+        <v>59</v>
+      </c>
+      <c r="J25" s="1">
+        <v>70</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
@@ -3177,739 +4106,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
-    <col min="2" max="2" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.109375" style="1"/>
-    <col min="5" max="5" width="11.5546875" style="1" customWidth="1"/>
-    <col min="6" max="6" width="11.6640625" style="1" customWidth="1"/>
-    <col min="7" max="8" width="11.44140625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.44140625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="5.44140625" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="1">
-        <f>SUMPRODUCT(doit,NPV)</f>
-        <v>9157</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E2" s="1">
-        <f t="shared" ref="E2:J2" si="0">SUMPRODUCT(doit,E6:E25)</f>
-        <v>2444</v>
-      </c>
-      <c r="F2" s="1">
-        <f t="shared" si="0"/>
-        <v>2760</v>
-      </c>
-      <c r="G2" s="1">
-        <f t="shared" si="0"/>
-        <v>2837</v>
-      </c>
-      <c r="H2" s="1">
-        <f t="shared" si="0"/>
-        <v>866</v>
-      </c>
-      <c r="I2" s="1">
-        <f t="shared" si="0"/>
-        <v>895</v>
-      </c>
-      <c r="J2" s="1">
-        <f t="shared" si="0"/>
-        <v>659</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="1">
-        <v>2500</v>
-      </c>
-      <c r="F4" s="1">
-        <v>2800</v>
-      </c>
-      <c r="G4" s="1">
-        <v>2900</v>
-      </c>
-      <c r="H4" s="1">
-        <v>900</v>
-      </c>
-      <c r="I4" s="1">
-        <v>900</v>
-      </c>
-      <c r="J4" s="1">
-        <v>900</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>0</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="1">
-        <v>928</v>
-      </c>
-      <c r="E6" s="1">
-        <v>398</v>
-      </c>
-      <c r="F6" s="1">
-        <v>180</v>
-      </c>
-      <c r="G6" s="1">
-        <v>368</v>
-      </c>
-      <c r="H6" s="1">
-        <v>111</v>
-      </c>
-      <c r="I6" s="1">
-        <v>108</v>
-      </c>
-      <c r="J6" s="1">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>1</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="1">
-        <v>908</v>
-      </c>
-      <c r="E7" s="1">
-        <v>151</v>
-      </c>
-      <c r="F7" s="1">
-        <v>269</v>
-      </c>
-      <c r="G7" s="1">
-        <v>248</v>
-      </c>
-      <c r="H7" s="1">
-        <v>139</v>
-      </c>
-      <c r="I7" s="1">
-        <v>86</v>
-      </c>
-      <c r="J7" s="1">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="1">
-        <v>801</v>
-      </c>
-      <c r="E8" s="1">
-        <v>129</v>
-      </c>
-      <c r="F8" s="1">
-        <v>189</v>
-      </c>
-      <c r="G8" s="1">
-        <v>308</v>
-      </c>
-      <c r="H8" s="1">
-        <v>56</v>
-      </c>
-      <c r="I8" s="1">
-        <v>61</v>
-      </c>
-      <c r="J8" s="1">
-        <v>23</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="1">
-        <v>543</v>
-      </c>
-      <c r="E9" s="1">
-        <v>275</v>
-      </c>
-      <c r="F9" s="1">
-        <v>218</v>
-      </c>
-      <c r="G9" s="1">
-        <v>220</v>
-      </c>
-      <c r="H9" s="1">
-        <v>54</v>
-      </c>
-      <c r="I9" s="1">
-        <v>70</v>
-      </c>
-      <c r="J9" s="1">
-        <v>59</v>
-      </c>
-      <c r="L9" s="1">
-        <f>A8</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>0</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" s="1">
-        <v>944</v>
-      </c>
-      <c r="E10" s="1">
-        <v>291</v>
-      </c>
-      <c r="F10" s="1">
-        <v>252</v>
-      </c>
-      <c r="G10" s="1">
-        <v>228</v>
-      </c>
-      <c r="H10" s="1">
-        <v>123</v>
-      </c>
-      <c r="I10" s="1">
-        <v>141</v>
-      </c>
-      <c r="J10" s="1">
-        <v>70</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>1</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="1">
-        <v>848</v>
-      </c>
-      <c r="E11" s="1">
-        <v>80</v>
-      </c>
-      <c r="F11" s="1">
-        <v>283</v>
-      </c>
-      <c r="G11" s="1">
-        <v>285</v>
-      </c>
-      <c r="H11" s="1">
-        <v>119</v>
-      </c>
-      <c r="I11" s="1">
-        <v>84</v>
-      </c>
-      <c r="J11" s="1">
-        <v>37</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>1</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="1">
-        <v>545</v>
-      </c>
-      <c r="E12" s="1">
-        <v>203</v>
-      </c>
-      <c r="F12" s="1">
-        <v>220</v>
-      </c>
-      <c r="G12" s="1">
-        <v>77</v>
-      </c>
-      <c r="H12" s="1">
-        <v>54</v>
-      </c>
-      <c r="I12" s="1">
-        <v>44</v>
-      </c>
-      <c r="J12" s="1">
-        <v>42</v>
-      </c>
-      <c r="L12" s="1">
-        <f>A9</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
-        <v>1</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C13" s="1">
-        <v>808</v>
-      </c>
-      <c r="E13" s="1">
-        <v>150</v>
-      </c>
-      <c r="F13" s="1">
-        <v>113</v>
-      </c>
-      <c r="G13" s="1">
-        <v>143</v>
-      </c>
-      <c r="H13" s="1">
-        <v>67</v>
-      </c>
-      <c r="I13" s="1">
-        <v>101</v>
-      </c>
-      <c r="J13" s="1">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>1</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="1">
-        <v>638</v>
-      </c>
-      <c r="E14" s="1">
-        <v>282</v>
-      </c>
-      <c r="F14" s="1">
-        <v>141</v>
-      </c>
-      <c r="G14" s="1">
-        <v>160</v>
-      </c>
-      <c r="H14" s="1">
-        <v>37</v>
-      </c>
-      <c r="I14" s="1">
-        <v>55</v>
-      </c>
-      <c r="J14" s="1">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
-        <v>0</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="1">
-        <v>841</v>
-      </c>
-      <c r="E15" s="1">
-        <v>214</v>
-      </c>
-      <c r="F15" s="1">
-        <v>254</v>
-      </c>
-      <c r="G15" s="1">
-        <v>355</v>
-      </c>
-      <c r="H15" s="1">
-        <v>130</v>
-      </c>
-      <c r="I15" s="1">
-        <v>72</v>
-      </c>
-      <c r="J15" s="1">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>0</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="1">
-        <v>664</v>
-      </c>
-      <c r="E16" s="1">
-        <v>224</v>
-      </c>
-      <c r="F16" s="1">
-        <v>271</v>
-      </c>
-      <c r="G16" s="1">
-        <v>130</v>
-      </c>
-      <c r="H16" s="1">
-        <v>51</v>
-      </c>
-      <c r="I16" s="1">
-        <v>79</v>
-      </c>
-      <c r="J16" s="1">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
-        <v>0</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="1">
-        <v>546</v>
-      </c>
-      <c r="E17" s="1">
-        <v>225</v>
-      </c>
-      <c r="F17" s="1">
-        <v>150</v>
-      </c>
-      <c r="G17" s="1">
-        <v>33</v>
-      </c>
-      <c r="H17" s="1">
-        <v>35</v>
-      </c>
-      <c r="I17" s="1">
-        <v>107</v>
-      </c>
-      <c r="J17" s="1">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
-        <v>0</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="1">
-        <v>699</v>
-      </c>
-      <c r="E18" s="1">
-        <v>101</v>
-      </c>
-      <c r="F18" s="1">
-        <v>218</v>
-      </c>
-      <c r="G18" s="1">
-        <v>272</v>
-      </c>
-      <c r="H18" s="1">
-        <v>43</v>
-      </c>
-      <c r="I18" s="1">
-        <v>90</v>
-      </c>
-      <c r="J18" s="1">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
-        <v>0</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" s="1">
-        <v>599</v>
-      </c>
-      <c r="E19" s="1">
-        <v>255</v>
-      </c>
-      <c r="F19" s="1">
-        <v>202</v>
-      </c>
-      <c r="G19" s="1">
-        <v>70</v>
-      </c>
-      <c r="H19" s="1">
-        <v>3</v>
-      </c>
-      <c r="I19" s="1">
-        <v>75</v>
-      </c>
-      <c r="J19" s="1">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
-        <v>1</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20" s="1">
-        <v>903</v>
-      </c>
-      <c r="E20" s="1">
-        <v>228</v>
-      </c>
-      <c r="F20" s="1">
-        <v>351</v>
-      </c>
-      <c r="G20" s="1">
-        <v>240</v>
-      </c>
-      <c r="H20" s="1">
-        <v>60</v>
-      </c>
-      <c r="I20" s="1">
-        <v>93</v>
-      </c>
-      <c r="J20" s="1">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>1</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C21" s="1">
-        <v>859</v>
-      </c>
-      <c r="E21" s="1">
-        <v>303</v>
-      </c>
-      <c r="F21" s="1">
-        <v>173</v>
-      </c>
-      <c r="G21" s="1">
-        <v>431</v>
-      </c>
-      <c r="H21" s="1">
-        <v>60</v>
-      </c>
-      <c r="I21" s="1">
-        <v>90</v>
-      </c>
-      <c r="J21" s="1">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>1</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="1">
-        <v>748</v>
-      </c>
-      <c r="E22" s="1">
-        <v>133</v>
-      </c>
-      <c r="F22" s="1">
-        <v>427</v>
-      </c>
-      <c r="G22" s="1">
-        <v>220</v>
-      </c>
-      <c r="H22" s="1">
-        <v>59</v>
-      </c>
-      <c r="I22" s="1">
-        <v>40</v>
-      </c>
-      <c r="J22" s="1">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>1</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C23" s="1">
-        <v>668</v>
-      </c>
-      <c r="E23" s="1">
-        <v>197</v>
-      </c>
-      <c r="F23" s="1">
-        <v>98</v>
-      </c>
-      <c r="G23" s="1">
-        <v>214</v>
-      </c>
-      <c r="H23" s="1">
-        <v>95</v>
-      </c>
-      <c r="I23" s="1">
-        <v>96</v>
-      </c>
-      <c r="J23" s="1">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>1</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="1">
-        <v>888</v>
-      </c>
-      <c r="E24" s="1">
-        <v>313</v>
-      </c>
-      <c r="F24" s="1">
-        <v>278</v>
-      </c>
-      <c r="G24" s="1">
-        <v>291</v>
-      </c>
-      <c r="H24" s="1">
-        <v>66</v>
-      </c>
-      <c r="I24" s="1">
-        <v>75</v>
-      </c>
-      <c r="J24" s="1">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>0</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="1">
-        <v>655</v>
-      </c>
-      <c r="E25" s="1">
-        <v>152</v>
-      </c>
-      <c r="F25" s="1">
-        <v>211</v>
-      </c>
-      <c r="G25" s="1">
-        <v>134</v>
-      </c>
-      <c r="H25" s="1">
-        <v>85</v>
-      </c>
-      <c r="I25" s="1">
-        <v>59</v>
-      </c>
-      <c r="J25" s="1">
-        <v>70</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
@@ -3944,23 +4140,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
-  <documentManagement>
-    <Used_x0020_in_x0020_Chapter xmlns="d1607db4-bd3f-4f82-a312-bf7e283d0a6b">true</Used_x0020_in_x0020_Chapter>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100AF8E4BBD310ADB419B3C5F1ACE4D113D" ma:contentTypeVersion="1" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="63e1bd94a874076348984a0131457edc">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d1607db4-bd3f-4f82-a312-bf7e283d0a6b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7c9989741aedae2f07a76d9f40ef2a18" ns2:_="">
     <xsd:import namespace="d1607db4-bd3f-4f82-a312-bf7e283d0a6b"/>
@@ -4020,30 +4199,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{485DC2A9-352C-42ED-81BC-D7BBDD9203A0}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="d1607db4-bd3f-4f82-a312-bf7e283d0a6b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEB10027-9737-4A22-84C4-CF7075237DC1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance">
+  <documentManagement>
+    <Used_x0020_in_x0020_Chapter xmlns="d1607db4-bd3f-4f82-a312-bf7e283d0a6b">true</Used_x0020_in_x0020_Chapter>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{85831C22-D7A3-44E1-A019-BC833F45315A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4058,4 +4231,27 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/internal/2005/internalDocumentation"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FEB10027-9737-4A22-84C4-CF7075237DC1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{485DC2A9-352C-42ED-81BC-D7BBDD9203A0}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="d1607db4-bd3f-4f82-a312-bf7e283d0a6b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>